<commit_message>
Major changes to examples, to have spectra_filetype, and spectra_file_ext and meta_file_ext
</commit_message>
<xml_diff>
--- a/docs/Examples/Fitting_Fermi_Diads/Example1a_Gas_Cell_Calibration/Strong_Diads.xlsx
+++ b/docs/Examples/Fitting_Fermi_Diads/Example1a_Gas_Cell_Calibration/Strong_Diads.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM41"/>
+  <dimension ref="A1:AW41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,6 +629,56 @@
           <t>Diad1_Gauss_Sigma</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Asym50</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Asym70</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Yuan2017_sym_factor</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_Remigi2021_BSF</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Asym50</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Asym70</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Yuan2017_sym_factor</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_Remigi2021_BSF</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Diad1_PDF_Model</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Diad2_PDF_Model</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -754,6 +804,40 @@
       <c r="AM2" t="n">
         <v>23.86975592865199</v>
       </c>
+      <c r="AN2" t="n">
+        <v>1.03924418604628</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>1.067524115755621</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.09294992267102321</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.001174360047450375</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>1.027829313543406</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1.036486486486378</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.05110870646721</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.0004494362872095745</v>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -879,6 +963,40 @@
       <c r="AM3" t="n">
         <v>21.56756763898271</v>
       </c>
+      <c r="AN3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>1.057359307359355</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.002494690735765187</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1.007407407407174</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>1.006666666666859</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.01355159393319092</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.000986424201431185</v>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1004,6 +1122,40 @@
       <c r="AM4" t="n">
         <v>12.02185666480601</v>
       </c>
+      <c r="AN4" t="n">
+        <v>1.065916398714034</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>1.079096045197823</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.1413521540883511</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>0.0001076211753072035</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>1.038016528925696</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>1.036951501154809</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.07845682919653348</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>5.386012680052075e-05</v>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1129,6 +1281,40 @@
       <c r="AM5" t="n">
         <v>11.98801775640944</v>
       </c>
+      <c r="AN5" t="n">
+        <v>1.008928571428609</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1.03205128205142</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.020260190675305</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.0005909207691690525</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1.042179261863007</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1.027295285359856</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.0822473557347556</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.0002553284101712544</v>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1254,6 +1440,40 @@
       <c r="AM6" t="n">
         <v>17.69947081273979</v>
       </c>
+      <c r="AN6" t="n">
+        <v>1.024817518248215</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>1.050847457627338</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.05797172548690677</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.0007344307610846852</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>1.042857142856986</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>1.036432160803926</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.08263645535369156</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.0002980204416081911</v>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1379,6 +1599,40 @@
       <c r="AM7" t="n">
         <v>19.75462087789007</v>
       </c>
+      <c r="AN7" t="n">
+        <v>1.056851311953394</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>1.060796645702328</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.1351226812812126</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.00055484347355365</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>1.007017543859899</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>1.009950248756407</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.01358323277711277</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.0002215351849421712</v>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1504,6 +1758,40 @@
       <c r="AM8" t="n">
         <v>20.19877015295504</v>
       </c>
+      <c r="AN8" t="n">
+        <v>1.028571428571292</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>1.040164778578815</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0.06842606293422047</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.0005970437511331655</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>1.007005253940234</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>1.001236093943142</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.01359184875204039</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.0002348081589615916</v>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1629,6 +1917,40 @@
       <c r="AM9" t="n">
         <v>20.8122053967793</v>
       </c>
+      <c r="AN9" t="n">
+        <v>1.025387870239883</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>1.03245436105486</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.06151390447886592</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.0006513373828178233</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>1.017667844523006</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>1.01500000000003</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.03416633629309355</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.0002511874768387845</v>
+      </c>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1754,6 +2076,40 @@
       <c r="AM10" t="n">
         <v>19.94667945161834</v>
       </c>
+      <c r="AN10" t="n">
+        <v>1.005563282336478</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>1.012072434607832</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>0.01349393722169638</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.0006957388697993795</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>1.021164021163825</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>1.015056461731523</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.04094331956343265</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.0002702021185361417</v>
+      </c>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1879,6 +2235,40 @@
       <c r="AM11" t="n">
         <v>20.76924366484819</v>
       </c>
+      <c r="AN11" t="n">
+        <v>1.012413793103315</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>1.031218529707996</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.03048133290426343</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.0007682889621280452</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>1.019332161687447</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>1.020075282308698</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.03748927363041101</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.000294244433819428</v>
+      </c>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2003,6 +2393,40 @@
       </c>
       <c r="AM12" t="n">
         <v>21.6391934309728</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>1.004103967168464</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>1.017874875868992</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.01015601766420204</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.0008425308340448408</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>1.040780141843812</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>1.015037593984825</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.07892957832104637</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.0003187259645000696</v>
+      </c>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2123,6 +2547,40 @@
       <c r="AM13" t="n">
         <v>21.5792614718319</v>
       </c>
+      <c r="AN13" t="n">
+        <v>1.006784260515389</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>1.006896551724079</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.01689956498825898</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.001043220757249656</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>1.021201413427365</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1.031887755101759</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0.0408239630457024</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.0003891599702277221</v>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2248,6 +2706,40 @@
       <c r="AM14" t="n">
         <v>22.19254465924697</v>
       </c>
+      <c r="AN14" t="n">
+        <v>1.034818941504008</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>1.072090628218265</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.08582528972555475</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.001178541364189213</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>1.04181818181802</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>1.055190538764714</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0.07933796137153437</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.0004423479971563969</v>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2373,6 +2865,40 @@
       <c r="AM15" t="n">
         <v>11.82106588807103</v>
       </c>
+      <c r="AN15" t="n">
+        <v>1.067632850241421</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>1.075963718820854</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.1449453244435877</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>7.062521825926832e-05</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>1.031404958677419</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>1.024193548387014</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0.06446635925383314</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>3.526512058950705e-05</v>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2498,6 +3024,40 @@
       <c r="AM16" t="n">
         <v>21.97384953470382</v>
       </c>
+      <c r="AN16" t="n">
+        <v>1.04571428571422</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>1.079533404029448</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.1103913797276458</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>0.001295651111235743</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>1.012820512820538</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>1.029372496662095</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0.02378292803230891</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.0004848755255659717</v>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2623,6 +3183,40 @@
       <c r="AM17" t="n">
         <v>23.96572017924257</v>
       </c>
+      <c r="AN17" t="n">
+        <v>1.110939907550138</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>1.121923937360291</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.2573763910679049</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>0.000896657592359939</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>1.015037593984993</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>1.032653061224743</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0.02725672736957571</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.0003455400358323411</v>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2748,6 +3342,40 @@
       <c r="AM18" t="n">
         <v>24.40546122070678</v>
       </c>
+      <c r="AN18" t="n">
+        <v>1.132686084142363</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>1.140208574739307</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0.2982823855060964</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0.0009049567607945373</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>1.034749034749107</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0.06165266724122178</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.000359507069031948</v>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2873,6 +3501,40 @@
       <c r="AM19" t="n">
         <v>24.08467252485052</v>
       </c>
+      <c r="AN19" t="n">
+        <v>1.082934609250165</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>1.111111111111059</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.1834642438586764</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.0009266803238578607</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>1.060362173038074</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>1.06926406926401</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0.104385412878888</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>0.0003622981235146658</v>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2998,6 +3660,40 @@
       <c r="AM20" t="n">
         <v>26.41823113371343</v>
       </c>
+      <c r="AN20" t="n">
+        <v>1.070607553366102</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>1.112048192771238</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>0.1509927321628118</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0.0009229406821181295</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>1.084710743802117</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>1.083209509658628</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0.1437428372662998</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.0003724244786045991</v>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3123,6 +3819,40 @@
       <c r="AM21" t="n">
         <v>25.80458930425644</v>
       </c>
+      <c r="AN21" t="n">
+        <v>1.135325131809961</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>1.123915737298542</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>0.2803858972116012</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0.0009003671816439495</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>1.066390041493627</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>1.070359281437066</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0.1112180085019031</v>
+      </c>
+      <c r="AU21" t="n">
+        <v>0.0003775535404007034</v>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3248,6 +3978,40 @@
       <c r="AM22" t="n">
         <v>24.92446196351823</v>
       </c>
+      <c r="AN22" t="n">
+        <v>1.011965811965708</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>1.049382716049311</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>0.0239544444159085</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0.0008628845090370497</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>1.077419354838866</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>1.072981366459779</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0.125847171837782</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>0.0003662685398816467</v>
+      </c>
+      <c r="AV22" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW22" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3373,6 +4137,40 @@
       <c r="AM23" t="n">
         <v>24.61100448908055</v>
       </c>
+      <c r="AN23" t="n">
+        <v>1.060283687943362</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>1.104113110539944</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>0.1191797163816126</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>0.0007669237727860179</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>1.057692307691835</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>1.044478527607034</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0.09360107500556623</v>
+      </c>
+      <c r="AU23" t="n">
+        <v>0.0003324066635493504</v>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3498,6 +4296,40 @@
       <c r="AM24" t="n">
         <v>22.67832199643803</v>
       </c>
+      <c r="AN24" t="n">
+        <v>1.011299435028042</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>1.025780189959096</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>0.02056635318386869</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>0.0007445231293312656</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>1.045351473922682</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>1.02442996742654</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>0.06904949671006134</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>0.0003359305525530544</v>
+      </c>
+      <c r="AV24" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW24" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3623,6 +4455,40 @@
       <c r="AM25" t="n">
         <v>21.07078434692326</v>
       </c>
+      <c r="AN25" t="n">
+        <v>1.044897959183957</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>1.034985422740475</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>0.07590025335372035</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0.0007490718126904229</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>1.092857142857002</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>1.0634648370494</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0.1365624470357426</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>0.0003614294069522319</v>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3748,6 +4614,40 @@
       <c r="AM26" t="n">
         <v>11.37541844361838</v>
       </c>
+      <c r="AN26" t="n">
+        <v>1.043130990415523</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>1.064406779661139</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>0.09259896113959688</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>7.194899821363043e-05</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>1.021594684385425</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>1.018626309662436</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0.04411200634865909</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>3.571223055933054e-05</v>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3873,6 +4773,40 @@
       <c r="AM27" t="n">
         <v>20.48240256168662</v>
       </c>
+      <c r="AN27" t="n">
+        <v>1.012422360248499</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>1.010416666666577</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>0.02040516070129824</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0.000799021250840475</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>1.055155875299545</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>1.049209138839928</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0.07843608075497685</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>0.0003834799969864633</v>
+      </c>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3998,6 +4932,40 @@
       <c r="AM28" t="n">
         <v>19.10386242222128</v>
       </c>
+      <c r="AN28" t="n">
+        <v>1.04260089686127</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>1.027914614121554</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>0.06522544977553869</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>0.0002165228514196018</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>1.068354430379547</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>1.010948905109266</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0.09290746995222129</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>0.0001118777191081769</v>
+      </c>
+      <c r="AV28" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4123,6 +5091,40 @@
       <c r="AM29" t="n">
         <v>18.39004995211761</v>
       </c>
+      <c r="AN29" t="n">
+        <v>1.092417061611448</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>1.060240963855369</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>0.1362490163715074</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>0.0002382452540167413</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>1.05897435897448</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>1.007393715341974</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0.07929859589615564</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>0.0001308179255665627</v>
+      </c>
+      <c r="AV29" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4248,6 +5250,40 @@
       <c r="AM30" t="n">
         <v>17.77074909103529</v>
       </c>
+      <c r="AN30" t="n">
+        <v>1.095121951219927</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>1.086175942549752</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>0.1354903860035039</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>0.000291932537666874</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>1.020671834625013</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>1.009469696969716</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0.02717822835923683</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>0.0001665158222054262</v>
+      </c>
+      <c r="AV30" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4373,6 +5409,40 @@
       <c r="AM31" t="n">
         <v>17.22719723084757</v>
       </c>
+      <c r="AN31" t="n">
+        <v>1.012048192771353</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>1.056880733945033</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>0.01662740244724191</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>0.0003227444916612971</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>1.044854881266586</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>1.046875000000098</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0.05837634682084049</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>0.000192009718655885</v>
+      </c>
+      <c r="AV31" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW31" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4498,6 +5568,40 @@
       <c r="AM32" t="n">
         <v>17.22944655437831</v>
       </c>
+      <c r="AN32" t="n">
+        <v>1.054590570719944</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>1.003610108302941</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>0.07532086641963574</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>0.0003701526931348638</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>1.102777777777597</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>1.08333333333322</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0.1304876387302916</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>0.0002152689846313107</v>
+      </c>
+      <c r="AV32" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW32" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4623,6 +5727,40 @@
       <c r="AM33" t="n">
         <v>16.71211058583604</v>
       </c>
+      <c r="AN33" t="n">
+        <v>1.046272493573117</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>1.013108614232349</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>0.06190972502839603</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>0.0004191749838900404</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>1.146131805157929</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>1.117894736842371</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0.1817453663788892</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>0.000252321633345186</v>
+      </c>
+      <c r="AV33" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW33" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4748,6 +5886,40 @@
       <c r="AM34" t="n">
         <v>16.46849315606015</v>
       </c>
+      <c r="AN34" t="n">
+        <v>1.015463917526187</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>1.04826254826258</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>0.02038689123887979</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>0.0005390164499805197</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>1.147398843930534</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>1.118279569892423</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>0.1800121861842587</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>0.0003169490326684566</v>
+      </c>
+      <c r="AV34" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW34" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4873,6 +6045,40 @@
       <c r="AM35" t="n">
         <v>16.29555216846881</v>
       </c>
+      <c r="AN35" t="n">
+        <v>1.066666666666333</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>1.073122529644124</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>0.08696589861624313</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>0.0005853884250909497</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>1.15652173913035</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>1.130151843817762</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>0.1911431265279137</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>0.000353830932445524</v>
+      </c>
+      <c r="AV35" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW35" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4998,6 +6204,40 @@
       <c r="AM36" t="n">
         <v>12.14850514880128</v>
       </c>
+      <c r="AN36" t="n">
+        <v>1.084415584415801</v>
+      </c>
+      <c r="AO36" t="n">
+        <v>1.090804597701284</v>
+      </c>
+      <c r="AP36" t="n">
+        <v>0.1816867867490985</v>
+      </c>
+      <c r="AQ36" t="n">
+        <v>7.450233908562922e-05</v>
+      </c>
+      <c r="AR36" t="n">
+        <v>1.006688963211165</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>1.005875440658219</v>
+      </c>
+      <c r="AT36" t="n">
+        <v>0.01352468680109353</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>3.643948909247885e-05</v>
+      </c>
+      <c r="AV36" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW36" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5123,6 +6363,40 @@
       <c r="AM37" t="n">
         <v>11.63088217772724</v>
       </c>
+      <c r="AN37" t="n">
+        <v>1.088709677419365</v>
+      </c>
+      <c r="AO37" t="n">
+        <v>1.098737083811603</v>
+      </c>
+      <c r="AP37" t="n">
+        <v>0.1920562401547117</v>
+      </c>
+      <c r="AQ37" t="n">
+        <v>7.551107355794174e-05</v>
+      </c>
+      <c r="AR37" t="n">
+        <v>1.005050505050515</v>
+      </c>
+      <c r="AS37" t="n">
+        <v>1.011890606420952</v>
+      </c>
+      <c r="AT37" t="n">
+        <v>0.01014048987562415</v>
+      </c>
+      <c r="AU37" t="n">
+        <v>3.622520542819809e-05</v>
+      </c>
+      <c r="AV37" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW37" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5248,6 +6522,40 @@
       <c r="AM38" t="n">
         <v>11.68000997385355</v>
       </c>
+      <c r="AN38" t="n">
+        <v>1.056962025316701</v>
+      </c>
+      <c r="AO38" t="n">
+        <v>1.073529411764971</v>
+      </c>
+      <c r="AP38" t="n">
+        <v>0.1238007423164539</v>
+      </c>
+      <c r="AQ38" t="n">
+        <v>7.815488535699481e-05</v>
+      </c>
+      <c r="AR38" t="n">
+        <v>1.017064846416417</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>1.020408163265185</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>0.03405991724451181</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>3.69901986453361e-05</v>
+      </c>
+      <c r="AV38" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW38" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5373,6 +6681,40 @@
       <c r="AM39" t="n">
         <v>11.89183658063558</v>
       </c>
+      <c r="AN39" t="n">
+        <v>1.020123839009232</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>1.05345211581284</v>
+      </c>
+      <c r="AP39" t="n">
+        <v>0.04413368996029979</v>
+      </c>
+      <c r="AQ39" t="n">
+        <v>8.404644855743969e-05</v>
+      </c>
+      <c r="AR39" t="n">
+        <v>1.022260273972824</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>1.02660217654188</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>0.04416302421903619</v>
+      </c>
+      <c r="AU39" t="n">
+        <v>3.899310420988014e-05</v>
+      </c>
+      <c r="AV39" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW39" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5498,6 +6840,40 @@
       <c r="AM40" t="n">
         <v>12.53059824357729</v>
       </c>
+      <c r="AN40" t="n">
+        <v>1.048437500000279</v>
+      </c>
+      <c r="AO40" t="n">
+        <v>1.077951002227406</v>
+      </c>
+      <c r="AP40" t="n">
+        <v>0.1072562951986242</v>
+      </c>
+      <c r="AQ40" t="n">
+        <v>0.0001484331488480449</v>
+      </c>
+      <c r="AR40" t="n">
+        <v>1.019031141868783</v>
+      </c>
+      <c r="AS40" t="n">
+        <v>1.017073170731907</v>
+      </c>
+      <c r="AT40" t="n">
+        <v>0.03730142248685587</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>6.6764468924883e-05</v>
+      </c>
+      <c r="AV40" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW40" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5622,6 +6998,40 @@
       </c>
       <c r="AM41" t="n">
         <v>11.69155883123316</v>
+      </c>
+      <c r="AN41" t="n">
+        <v>1.019969278033739</v>
+      </c>
+      <c r="AO41" t="n">
+        <v>1.058177826564262</v>
+      </c>
+      <c r="AP41" t="n">
+        <v>0.04424108498184742</v>
+      </c>
+      <c r="AQ41" t="n">
+        <v>0.0005608119883110123</v>
+      </c>
+      <c r="AR41" t="n">
+        <v>1.01379310344807</v>
+      </c>
+      <c r="AS41" t="n">
+        <v>1.017094017093887</v>
+      </c>
+      <c r="AT41" t="n">
+        <v>0.02703091809469135</v>
+      </c>
+      <c r="AU41" t="n">
+        <v>0.0002528881473847128</v>
+      </c>
+      <c r="AV41" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
+      </c>
+      <c r="AW41" t="inlineStr">
+        <is>
+          <t>PseudoVoigtModel</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>